<commit_message>
Excel Document and Screenshot Updated
</commit_message>
<xml_diff>
--- a/realestate/documents/RipartizioneSpeseImmobiliari.xlsx
+++ b/realestate/documents/RipartizioneSpeseImmobiliari.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bananach-my.sharepoint.com/personal/patrick_pasquillo_banana_ch/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrick.pasquillo\Documents\GitHub\Universal\realestate\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="8_{EB4C9B1F-70B0-486D-9782-699C190AD19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84F43644-0BCB-458E-A121-E4B0A1642545}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72333AEB-FEF6-4EB7-81DB-32FC245CD99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C8DA3664-E04A-4EE4-B0E8-18F2F24E5315}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -179,23 +179,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -203,14 +208,30 @@
   <dxfs count="11">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -229,7 +250,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -248,6 +270,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -266,6 +289,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -284,6 +308,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -302,6 +327,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -320,6 +346,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -338,26 +365,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="none"/>
+        <b/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -373,14 +386,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7EDFFC5C-15BA-41C1-A573-16895C48713E}" name="Tabella1" displayName="Tabella1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7EDFFC5C-15BA-41C1-A573-16895C48713E}" name="Tabella1" displayName="Tabella1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="10" dataDxfId="0">
   <autoFilter ref="A1:I13" xr:uid="{7EDFFC5C-15BA-41C1-A573-16895C48713E}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{2C273954-DE9B-4C1A-906F-88F1A8DE2F4E}" name="Spesa da ripartire" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{BDDF30DA-1A34-4AFE-8AC9-C4A5002891E6}" name="Saldo" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{F2EE9F63-F9A7-447D-B00D-397FB9B08280}" name="Coeff. app. 1" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{BA9C90F3-DDBF-49C0-B18F-A27C3F3C3441}" name="Coeff. app. 2" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{3B6004CA-EF77-449F-BDFC-540637EA9ACF}" name="Coeff. app. 3" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{2C273954-DE9B-4C1A-906F-88F1A8DE2F4E}" name="Spesa da ripartire" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{BDDF30DA-1A34-4AFE-8AC9-C4A5002891E6}" name="Saldo" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{F2EE9F63-F9A7-447D-B00D-397FB9B08280}" name="Coeff. app. 1" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{BA9C90F3-DDBF-49C0-B18F-A27C3F3C3441}" name="Coeff. app. 2" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{3B6004CA-EF77-449F-BDFC-540637EA9ACF}" name="Coeff. app. 3" dataDxfId="5"/>
     <tableColumn id="9" xr3:uid="{79589C4D-015B-4F0F-8BD0-7FD3B7996590}" name="Tot. Coeff." dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{CE2FA730-DC58-45E1-9E24-8CCE45FCA81E}" name="App. 1" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{1D501B41-CE35-4E48-95E4-C930E890E131}" name="App. 2" dataDxfId="2"/>
@@ -723,371 +736,376 @@
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>4000</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
         <v>54</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="5">
         <v>85</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="5">
         <v>124</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <f>$C2+$D2+$E2</f>
         <v>263</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <f>$B2/$F2*$C2</f>
         <v>821.29277566539929</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="6">
         <f>$B2/$F2*$D2</f>
         <v>1292.7756653992396</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <f>$B2/$F2*$E2</f>
         <v>1885.9315589353612</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>2000</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>54</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <v>85</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="5">
         <v>124</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <f t="shared" ref="F3:F11" si="0">$C3+$D3+$E3</f>
         <v>263</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="6">
         <f t="shared" ref="G3:G11" si="1">$B3/$F3*$C3</f>
         <v>410.64638783269965</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="6">
         <f t="shared" ref="H3:H11" si="2">$B3/$F3*$D3</f>
         <v>646.38783269961982</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="6">
         <f t="shared" ref="I3:I11" si="3">$B3/$F3*$E3</f>
         <v>942.96577946768059</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>200</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>54</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>85</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="5">
         <v>124</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <f t="shared" si="0"/>
         <v>263</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="6">
         <f t="shared" si="1"/>
         <v>41.064638783269956</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="6">
         <f t="shared" si="2"/>
         <v>64.638783269961976</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="6">
         <f t="shared" si="3"/>
         <v>94.296577946768053</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4">
         <v>50</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <v>54</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>85</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="5">
         <v>124</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>263</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="6">
         <f t="shared" si="1"/>
         <v>10.266159695817489</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="6">
         <f t="shared" si="2"/>
         <v>16.159695817490494</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="6">
         <f t="shared" si="3"/>
         <v>23.574144486692013</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="4">
         <v>800</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5">
         <v>54</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>85</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="5">
         <v>124</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>263</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <f t="shared" si="1"/>
         <v>164.25855513307982</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="6">
         <f t="shared" si="2"/>
         <v>258.55513307984791</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="6">
         <f t="shared" si="3"/>
         <v>377.18631178707221</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="4">
         <v>300</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="5">
         <v>54</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>85</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="5">
         <v>124</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>263</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="6">
         <f t="shared" si="1"/>
         <v>61.596958174904941</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="6">
         <f t="shared" si="2"/>
         <v>96.958174904942965</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="6">
         <f t="shared" si="3"/>
         <v>141.44486692015209</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="4">
         <v>400</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="5">
         <v>54</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="5">
         <v>85</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="5">
         <v>124</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>263</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
         <v>82.129277566539912</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="6">
         <f t="shared" si="2"/>
         <v>129.27756653992395</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="6">
         <f t="shared" si="3"/>
         <v>188.59315589353611</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="4">
         <v>500</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="5">
         <v>54</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <v>85</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="5">
         <v>124</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>263</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>102.66159695817491</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="6">
         <f t="shared" si="2"/>
         <v>161.59695817490496</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="6">
         <f t="shared" si="3"/>
         <v>235.74144486692015</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="4">
         <v>100</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="5">
         <v>54</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="5">
         <v>85</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="5">
         <v>124</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>263</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
         <v>20.532319391634978</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="6">
         <f t="shared" si="2"/>
         <v>32.319391634980988</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="6">
         <f t="shared" si="3"/>
         <v>47.148288973384027</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="4">
         <v>1250</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="5">
         <v>1</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>416.66666666666669</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="6">
         <f t="shared" si="2"/>
         <v>416.66666666666669</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="6">
         <f t="shared" si="3"/>
         <v>416.66666666666669</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="9">
-        <v>-1800</v>
+        <v>-2000</v>
       </c>
       <c r="H12" s="9">
         <v>-3000</v>
@@ -1096,19 +1114,24 @@
         <v>-4000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="6">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12">
         <f>SUM($G2:$G11)+$G12</f>
-        <v>331.11533586818769</v>
-      </c>
-      <c r="H13" s="6">
+        <v>131.11533586818769</v>
+      </c>
+      <c r="H13" s="12">
         <f>SUM($H2:$H11)+$H12</f>
         <v>115.33586818757931</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="12">
         <f>SUM($I2:$I11)+$I12</f>
         <v>353.54879594423346</v>
       </c>

</xml_diff>